<commit_message>
Update Industry and growth rates for fuels and BEV
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SUP_DomBioPot_SEAI.xlsx
+++ b/SuppXLS/Scen_B_SUP_DomBioPot_SEAI.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rbsul\Documents\GitHub\times-ireland-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB056EE-6DFE-4A7B-9B20-D27463A9AAF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB61F7F-F835-42CF-8A73-96C5B9968D03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5224,8 +5224,8 @@
   </sheetPr>
   <dimension ref="A1:DQ68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AZ9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BJ36" sqref="BJ36"/>
+    <sheetView tabSelected="1" topLeftCell="BE23" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="BQ38" sqref="BQ38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -13943,44 +13943,44 @@
         <v>3.3041335877500391</v>
       </c>
       <c r="BO31" s="97">
-        <f>H31/1000*Conversions!$B$2</f>
-        <v>0</v>
+        <f>+BN31</f>
+        <v>3.3041335877500391</v>
       </c>
       <c r="BP31" s="97">
-        <f>I31/1000*Conversions!$B$2</f>
-        <v>0</v>
+        <f t="shared" ref="BP31:BX31" si="10">+BO31</f>
+        <v>3.3041335877500391</v>
       </c>
       <c r="BQ31" s="97">
-        <f>J31/1000*Conversions!$B$2</f>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>3.3041335877500391</v>
       </c>
       <c r="BR31" s="97">
-        <f>K31/1000*Conversions!$B$2</f>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>3.3041335877500391</v>
       </c>
       <c r="BS31" s="97">
-        <f>L31/1000*Conversions!$B$2</f>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>3.3041335877500391</v>
       </c>
       <c r="BT31" s="97">
-        <f>M31/1000*Conversions!$B$2</f>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>3.3041335877500391</v>
       </c>
       <c r="BU31" s="97">
-        <f>N31/1000*Conversions!$B$2</f>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>3.3041335877500391</v>
       </c>
       <c r="BV31" s="97">
-        <f>O31/1000*Conversions!$B$2</f>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>3.3041335877500391</v>
       </c>
       <c r="BW31" s="97">
-        <f>P31/1000*Conversions!$B$2</f>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>3.3041335877500391</v>
       </c>
       <c r="BX31" s="97">
-        <f>Q31/1000*Conversions!$B$2</f>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>3.3041335877500391</v>
       </c>
       <c r="BY31" s="97">
         <f>SEAI!N24</f>
@@ -14364,7 +14364,7 @@
         <v>0.64080000000000004</v>
       </c>
       <c r="BX32" s="97">
-        <f t="shared" ref="BX32" si="10">BY32</f>
+        <f t="shared" ref="BX32" si="11">BY32</f>
         <v>0.64080000000000004</v>
       </c>
       <c r="BY32" s="97">
@@ -14745,11 +14745,11 @@
         <v>0.17682555599999999</v>
       </c>
       <c r="BW33" s="97">
-        <f t="shared" ref="BW33:BX33" si="11">BX33</f>
+        <f t="shared" ref="BW33:BX33" si="12">BX33</f>
         <v>0.18720000000000001</v>
       </c>
       <c r="BX33" s="97">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.18720000000000001</v>
       </c>
       <c r="BY33" s="97">
@@ -16288,47 +16288,47 @@
       <c r="BV37" s="64">
         <v>8</v>
       </c>
-      <c r="BW37" s="93">
-        <v>0</v>
-      </c>
-      <c r="BX37" s="93">
-        <v>0</v>
-      </c>
-      <c r="BY37" s="93">
-        <v>0</v>
-      </c>
-      <c r="BZ37" s="93">
-        <v>0</v>
-      </c>
-      <c r="CA37" s="93">
-        <v>0</v>
-      </c>
-      <c r="CB37" s="93">
-        <v>0</v>
-      </c>
-      <c r="CC37" s="93">
-        <v>0</v>
-      </c>
-      <c r="CD37" s="93">
-        <v>0</v>
-      </c>
-      <c r="CE37" s="93">
-        <v>0</v>
-      </c>
-      <c r="CF37" s="93">
-        <v>0</v>
-      </c>
-      <c r="CG37" s="93">
-        <v>0</v>
-      </c>
-      <c r="CH37" s="93">
-        <v>0</v>
-      </c>
-      <c r="CI37" s="93">
-        <v>0</v>
-      </c>
-      <c r="CJ37" s="93">
-        <v>0</v>
+      <c r="BW37" s="64">
+        <v>8</v>
+      </c>
+      <c r="BX37" s="64">
+        <v>8</v>
+      </c>
+      <c r="BY37" s="64">
+        <v>8</v>
+      </c>
+      <c r="BZ37" s="64">
+        <v>8</v>
+      </c>
+      <c r="CA37" s="64">
+        <v>8</v>
+      </c>
+      <c r="CB37" s="64">
+        <v>8</v>
+      </c>
+      <c r="CC37" s="64">
+        <v>8</v>
+      </c>
+      <c r="CD37" s="64">
+        <v>8</v>
+      </c>
+      <c r="CE37" s="64">
+        <v>8</v>
+      </c>
+      <c r="CF37" s="64">
+        <v>8</v>
+      </c>
+      <c r="CG37" s="64">
+        <v>8</v>
+      </c>
+      <c r="CH37" s="64">
+        <v>8</v>
+      </c>
+      <c r="CI37" s="64">
+        <v>8</v>
+      </c>
+      <c r="CJ37" s="64">
+        <v>8</v>
       </c>
       <c r="CK37" s="94">
         <v>5</v>
@@ -19606,11 +19606,11 @@
         <v>5</v>
       </c>
       <c r="CM50" s="11" t="str">
-        <f t="shared" ref="CM50:CM65" si="12">BG50</f>
+        <f t="shared" ref="CM50:CM65" si="13">BG50</f>
         <v>ABIOFRSR3</v>
       </c>
       <c r="CN50" s="11" t="str">
-        <f t="shared" ref="CN50:CN65" si="13">BH50</f>
+        <f t="shared" ref="CN50:CN65" si="14">BH50</f>
         <v>Forest thinnings - Hi</v>
       </c>
       <c r="CO50" t="s">
@@ -19620,7 +19620,7 @@
         <v>128</v>
       </c>
       <c r="CQ50" s="11" t="str">
-        <f t="shared" ref="CQ50:CQ65" si="14">BJ50</f>
+        <f t="shared" ref="CQ50:CQ65" si="15">BJ50</f>
         <v>BIOWOO</v>
       </c>
       <c r="CR50" s="11" t="s">
@@ -19898,7 +19898,7 @@
         <v>MINBIOWOO1_S3</v>
       </c>
       <c r="BH51" s="11" t="str">
-        <f t="shared" ref="BH51:BH65" si="15">A51</f>
+        <f t="shared" ref="BH51:BH65" si="16">A51</f>
         <v>Sawmill residues - Hi</v>
       </c>
       <c r="BI51" s="11" t="s">
@@ -19997,11 +19997,11 @@
         <v>5</v>
       </c>
       <c r="CM51" s="11" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>MINBIOWOO1_S3</v>
       </c>
       <c r="CN51" s="11" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Sawmill residues - Hi</v>
       </c>
       <c r="CO51" t="s">
@@ -20011,7 +20011,7 @@
         <v>128</v>
       </c>
       <c r="CQ51" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>BIOWOO</v>
       </c>
       <c r="CR51" s="11" t="s">
@@ -20290,7 +20290,7 @@
         <v>MINBIOWOO2_S3</v>
       </c>
       <c r="BH52" s="96" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>PCRW - Hi</v>
       </c>
       <c r="BI52" s="96" t="s">
@@ -20347,11 +20347,11 @@
         <v>0.28817857742882308</v>
       </c>
       <c r="BW52" s="97">
-        <f t="shared" ref="BW52:BX52" si="16">BX52</f>
+        <f t="shared" ref="BW52:BX52" si="17">BX52</f>
         <v>0.30599999999999999</v>
       </c>
       <c r="BX52" s="97">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.30599999999999999</v>
       </c>
       <c r="BY52" s="97">
@@ -20382,11 +20382,11 @@
         <v>5</v>
       </c>
       <c r="CM52" s="11" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>MINBIOWOO2_S3</v>
       </c>
       <c r="CN52" s="11" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>PCRW - Hi</v>
       </c>
       <c r="CO52" t="s">
@@ -20396,7 +20396,7 @@
         <v>128</v>
       </c>
       <c r="CQ52" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>BIOWOO</v>
       </c>
       <c r="CR52" s="11" t="s">
@@ -20674,7 +20674,7 @@
         <v>MINBIOMSW1_S3</v>
       </c>
       <c r="BH53" s="96" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Solid BMSW - Hi</v>
       </c>
       <c r="BI53" s="96" t="s">
@@ -20731,11 +20731,11 @@
         <v>0</v>
       </c>
       <c r="BW53" s="97">
-        <f t="shared" ref="BW53:BX53" si="17">BX53</f>
+        <f t="shared" ref="BW53:BX53" si="18">BX53</f>
         <v>0.24840000000000001</v>
       </c>
       <c r="BX53" s="97">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.24840000000000001</v>
       </c>
       <c r="BY53" s="97">
@@ -20766,11 +20766,11 @@
         <v>5</v>
       </c>
       <c r="CM53" s="11" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>MINBIOMSW1_S3</v>
       </c>
       <c r="CN53" s="11" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Solid BMSW - Hi</v>
       </c>
       <c r="CO53" t="s">
@@ -20780,7 +20780,7 @@
         <v>128</v>
       </c>
       <c r="CQ53" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>BIOMUN</v>
       </c>
       <c r="CR53" s="11" t="s">
@@ -21059,7 +21059,7 @@
         <v>MINBIOTLW_S3</v>
       </c>
       <c r="BH54" s="96" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Tallow - Hi</v>
       </c>
       <c r="BI54" s="96" t="s">
@@ -21116,11 +21116,11 @@
         <v>1.1185514173676627</v>
       </c>
       <c r="BW54" s="97">
-        <f t="shared" ref="BW54:BX54" si="18">BX54</f>
+        <f t="shared" ref="BW54:BX54" si="19">BX54</f>
         <v>1.1807999999999998</v>
       </c>
       <c r="BX54" s="97">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1.1807999999999998</v>
       </c>
       <c r="BY54" s="97">
@@ -21151,11 +21151,11 @@
         <v>5</v>
       </c>
       <c r="CM54" s="11" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>MINBIOTLW_S3</v>
       </c>
       <c r="CN54" s="11" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Tallow - Hi</v>
       </c>
       <c r="CO54" t="s">
@@ -21165,7 +21165,7 @@
         <v>128</v>
       </c>
       <c r="CQ54" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>BIOWOO</v>
       </c>
       <c r="CR54" s="11" t="s">
@@ -21443,7 +21443,7 @@
         <v>MINBIORVO_S3</v>
       </c>
       <c r="BH55" s="96" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>RVO - Hi</v>
       </c>
       <c r="BI55" s="96" t="s">
@@ -21500,11 +21500,11 @@
         <v>0</v>
       </c>
       <c r="BW55" s="97">
-        <f t="shared" ref="BW55:BX55" si="19">BX55</f>
+        <f t="shared" ref="BW55:BX55" si="20">BX55</f>
         <v>0</v>
       </c>
       <c r="BX55" s="97">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="BY55" s="97">
@@ -21531,11 +21531,11 @@
         <v>5</v>
       </c>
       <c r="CM55" s="11" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>MINBIORVO_S3</v>
       </c>
       <c r="CN55" s="11" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>RVO - Hi</v>
       </c>
       <c r="CO55" t="s">
@@ -21545,7 +21545,7 @@
         <v>128</v>
       </c>
       <c r="CQ55" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>BIORPS</v>
       </c>
       <c r="CR55" s="11" t="s">
@@ -21823,7 +21823,7 @@
         <v>MINBIOWOO3_S3</v>
       </c>
       <c r="BH56" s="96" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Straw - Hi</v>
       </c>
       <c r="BI56" s="96" t="s">
@@ -21915,11 +21915,11 @@
         <v>5</v>
       </c>
       <c r="CM56" s="11" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>MINBIOWOO3_S3</v>
       </c>
       <c r="CN56" s="11" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Straw - Hi</v>
       </c>
       <c r="CO56" t="s">
@@ -21929,7 +21929,7 @@
         <v>128</v>
       </c>
       <c r="CQ56" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>BIOWOO</v>
       </c>
       <c r="CR56" s="11" t="s">
@@ -22207,7 +22207,7 @@
         <v>MINBIOCATW_S3</v>
       </c>
       <c r="BH57" s="11" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Cattle waste - Hi</v>
       </c>
       <c r="BI57" s="11" t="s">
@@ -22306,11 +22306,11 @@
         <v>5</v>
       </c>
       <c r="CM57" s="11" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>MINBIOCATW_S3</v>
       </c>
       <c r="CN57" s="11" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Cattle waste - Hi</v>
       </c>
       <c r="CO57" t="s">
@@ -22320,7 +22320,7 @@
         <v>128</v>
       </c>
       <c r="CQ57" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>BIOSLU</v>
       </c>
       <c r="CR57" s="11" t="s">
@@ -22598,7 +22598,7 @@
         <v>MINBIOPIGW_S3</v>
       </c>
       <c r="BH58" s="11" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Pig waste - Hi</v>
       </c>
       <c r="BI58" s="11" t="s">
@@ -22697,11 +22697,11 @@
         <v>5</v>
       </c>
       <c r="CM58" s="11" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>MINBIOPIGW_S3</v>
       </c>
       <c r="CN58" s="11" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Pig waste - Hi</v>
       </c>
       <c r="CO58" t="s">
@@ -22711,7 +22711,7 @@
         <v>128</v>
       </c>
       <c r="CQ58" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>BIOSLU</v>
       </c>
       <c r="CR58" s="11" t="s">
@@ -22990,7 +22990,7 @@
         <v>MINBIOMSW2_S3</v>
       </c>
       <c r="BH59" s="11" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>BMSW - Hi</v>
       </c>
       <c r="BI59" s="11" t="s">
@@ -23089,11 +23089,11 @@
         <v>5</v>
       </c>
       <c r="CM59" s="11" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>MINBIOMSW2_S3</v>
       </c>
       <c r="CN59" s="11" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>BMSW - Hi</v>
       </c>
       <c r="CO59" t="s">
@@ -23103,7 +23103,7 @@
         <v>128</v>
       </c>
       <c r="CQ59" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>BIOMUN</v>
       </c>
       <c r="CR59" s="11" t="s">
@@ -23382,7 +23382,7 @@
         <v>ABIOCRP43</v>
       </c>
       <c r="BH60" s="11" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Willow - Hi</v>
       </c>
       <c r="BI60" s="11" t="s">
@@ -23481,11 +23481,11 @@
         <v>5</v>
       </c>
       <c r="CM60" s="11" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>ABIOCRP43</v>
       </c>
       <c r="CN60" s="11" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Willow - Hi</v>
       </c>
       <c r="CO60" t="s">
@@ -23495,7 +23495,7 @@
         <v>128</v>
       </c>
       <c r="CQ60" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>BIOWOO</v>
       </c>
       <c r="CR60" s="11" t="s">
@@ -23774,7 +23774,7 @@
         <v>ABIOCRP33</v>
       </c>
       <c r="BH61" s="11" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Miscanthus - Hi</v>
       </c>
       <c r="BI61" s="11" t="s">
@@ -23873,11 +23873,11 @@
         <v>5</v>
       </c>
       <c r="CM61" s="11" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>ABIOCRP33</v>
       </c>
       <c r="CN61" s="11" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Miscanthus - Hi</v>
       </c>
       <c r="CO61" t="s">
@@ -23887,7 +23887,7 @@
         <v>128</v>
       </c>
       <c r="CQ61" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>BIOWOO</v>
       </c>
       <c r="CR61" s="11" t="s">
@@ -24166,7 +24166,7 @@
         <v>ABIOCRP13</v>
       </c>
       <c r="BH62" s="11" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Wheat - Hi</v>
       </c>
       <c r="BI62" s="11" t="s">
@@ -24265,11 +24265,11 @@
         <v>5</v>
       </c>
       <c r="CM62" s="11" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>ABIOCRP13</v>
       </c>
       <c r="CN62" s="11" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Wheat - Hi</v>
       </c>
       <c r="CO62" t="s">
@@ -24279,7 +24279,7 @@
         <v>128</v>
       </c>
       <c r="CQ62" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>BIOCRP1</v>
       </c>
       <c r="CR62" s="11" t="s">
@@ -24558,7 +24558,7 @@
         <v>ABIOCRP23</v>
       </c>
       <c r="BH63" s="11" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>OSR - Hi</v>
       </c>
       <c r="BI63" s="11" t="s">
@@ -24657,11 +24657,11 @@
         <v>5</v>
       </c>
       <c r="CM63" s="11" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>ABIOCRP23</v>
       </c>
       <c r="CN63" s="11" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>OSR - Hi</v>
       </c>
       <c r="CO63" t="s">
@@ -24671,7 +24671,7 @@
         <v>128</v>
       </c>
       <c r="CQ63" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>BIORPS</v>
       </c>
       <c r="CR63" s="11" t="s">
@@ -24950,7 +24950,7 @@
         <v>ABIOGAS13</v>
       </c>
       <c r="BH64" s="96" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Crops Anaerobic - Hi</v>
       </c>
       <c r="BI64" s="96" t="s">
@@ -25041,11 +25041,11 @@
         <v>5</v>
       </c>
       <c r="CM64" s="11" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>ABIOGAS13</v>
       </c>
       <c r="CN64" s="11" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Crops Anaerobic - Hi</v>
       </c>
       <c r="CO64" t="s">
@@ -25055,7 +25055,7 @@
         <v>128</v>
       </c>
       <c r="CQ64" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>BIOGAS</v>
       </c>
       <c r="CR64" s="11" t="s">
@@ -25333,7 +25333,7 @@
         <v>MINBIOINDF_S3</v>
       </c>
       <c r="BH65" s="11" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Industrial Food - Hi</v>
       </c>
       <c r="BI65" s="11" t="s">
@@ -25432,11 +25432,11 @@
         <v>5</v>
       </c>
       <c r="CM65" s="11" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>MINBIOINDF_S3</v>
       </c>
       <c r="CN65" s="11" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Industrial Food - Hi</v>
       </c>
       <c r="CO65" t="s">
@@ -25446,7 +25446,7 @@
         <v>128</v>
       </c>
       <c r="CQ65" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>BIOSLU</v>
       </c>
       <c r="CR65" s="11" t="s">
@@ -25613,7 +25613,7 @@
     <row r="67" spans="1:121">
       <c r="CJ67" s="58">
         <f>SUM(CJ6:CJ21,CJ28:CJ43,CJ50:CJ65)</f>
-        <v>58.410000000000004</v>
+        <v>66.410000000000011</v>
       </c>
       <c r="CK67" s="11" t="s">
         <v>1</v>
@@ -25627,7 +25627,7 @@
       <c r="BC68" s="15"/>
       <c r="CJ68" s="58">
         <f>CJ67*1000/Conversions!$B$2</f>
-        <v>1395098.8822012038</v>
+        <v>1586175.5995032007</v>
       </c>
       <c r="CK68" s="11" t="s">
         <v>19</v>

</xml_diff>